<commit_message>
[@tomclement] Add checking for purchase order items and waybill items in e2e tests
</commit_message>
<xml_diff>
--- a/eums/client/test/functional/files/release-orders.xlsx
+++ b/eums/client/test/functional/files/release-orders.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="194">
   <si>
     <t>54102852</t>
   </si>
@@ -523,6 +523,84 @@
   </si>
   <si>
     <t>Volume in M3</t>
+  </si>
+  <si>
+    <t>54119455</t>
+  </si>
+  <si>
+    <t>SL002247</t>
+  </si>
+  <si>
+    <t>Computer, laptop</t>
+  </si>
+  <si>
+    <t>L438000617</t>
+  </si>
+  <si>
+    <t>Transcultual Psychosocial Organisation</t>
+  </si>
+  <si>
+    <t>Peter Krouwel</t>
+  </si>
+  <si>
+    <t>20158279</t>
+  </si>
+  <si>
+    <t>81025778</t>
+  </si>
+  <si>
+    <t>56181855</t>
+  </si>
+  <si>
+    <t>SM140426</t>
+  </si>
+  <si>
+    <t>4380/A0/04/107/004/020</t>
+  </si>
+  <si>
+    <t>3313</t>
+  </si>
+  <si>
+    <t>72095454</t>
+  </si>
+  <si>
+    <t>Marianna Garofalo</t>
+  </si>
+  <si>
+    <t>4900002391</t>
+  </si>
+  <si>
+    <t>SYS0116908</t>
+  </si>
+  <si>
+    <t>UAJ 076Y</t>
+  </si>
+  <si>
+    <t>Beneficiary collect</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>SL002248</t>
+  </si>
+  <si>
+    <t>Laptop bag</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>SYS0116909</t>
+  </si>
+  <si>
+    <t>SL006071</t>
+  </si>
+  <si>
+    <t>IT Accessories</t>
+  </si>
+  <si>
+    <t>SYS0116910</t>
   </si>
 </sst>
 </file>
@@ -545,12 +623,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -586,12 +670,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -610,6 +694,21 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
@@ -943,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BW7"/>
+  <dimension ref="A1:BW10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2514,6 +2613,663 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:75" s="9" customFormat="1">
+      <c r="A8" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10">
+        <v>42013</v>
+      </c>
+      <c r="D8" s="10">
+        <v>42013</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G8" s="11">
+        <v>3</v>
+      </c>
+      <c r="H8" s="12">
+        <v>3091.26</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE8" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF8" s="12">
+        <v>1022.75</v>
+      </c>
+      <c r="AG8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL8" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN8" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AO8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AU8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AV8" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AX8" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="AY8" s="10"/>
+      <c r="AZ8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BA8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BB8" s="10"/>
+      <c r="BC8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BD8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BE8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BF8" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BG8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BH8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="BI8" s="10"/>
+      <c r="BJ8" s="10"/>
+      <c r="BK8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BL8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BN8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BO8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ8" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="BR8" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="BS8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BT8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BU8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BV8" s="13">
+        <v>0</v>
+      </c>
+      <c r="BW8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:75" s="9" customFormat="1">
+      <c r="A9" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C9" s="10">
+        <v>42013</v>
+      </c>
+      <c r="D9" s="10">
+        <v>42013</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" s="11">
+        <v>3</v>
+      </c>
+      <c r="H9" s="12">
+        <v>104.01</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U9" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="Z9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF9" s="12">
+        <v>954.38</v>
+      </c>
+      <c r="AG9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN9" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AO9" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP9" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="AQ9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR9" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="AS9" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="AT9" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="AU9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AV9" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW9" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX9" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="AY9" s="10"/>
+      <c r="AZ9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BA9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BB9" s="10"/>
+      <c r="BC9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BD9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BE9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BF9" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BG9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BH9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="BI9" s="10"/>
+      <c r="BJ9" s="10"/>
+      <c r="BK9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BL9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BN9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BO9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ9" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="BR9" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="BS9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BT9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BU9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BV9" s="13">
+        <v>0</v>
+      </c>
+      <c r="BW9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:75" s="9" customFormat="1">
+      <c r="A10" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="10">
+        <v>42013</v>
+      </c>
+      <c r="D10" s="10">
+        <v>42013</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="11">
+        <v>3</v>
+      </c>
+      <c r="H10" s="12">
+        <v>124.84</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="R10" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="W10" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="X10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="Z10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF10" s="12">
+        <v>41.62</v>
+      </c>
+      <c r="AG10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="AM10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AN10" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="AO10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AU10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AV10" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="AW10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX10" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="AY10" s="10"/>
+      <c r="AZ10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BA10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BB10" s="10"/>
+      <c r="BC10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BD10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BE10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BF10" s="10">
+        <v>42016</v>
+      </c>
+      <c r="BG10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BH10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="BI10" s="10"/>
+      <c r="BJ10" s="10"/>
+      <c r="BK10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BL10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BM10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BN10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BO10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BP10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ10" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="BR10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="BS10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BT10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BU10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="BV10" s="13">
+        <v>0</v>
+      </c>
+      <c r="BW10" s="13">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>